<commit_message>
Fim da aula 2
</commit_message>
<xml_diff>
--- a/Ficha1/TabelaComCaracteristicasDasClasses.xlsx
+++ b/Ficha1/TabelaComCaracteristicasDasClasses.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpmf/MEOCloud/ESTG/P2/2017_2018/Praticas/PL-Ficha1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escola\Licenciatura\1º Ano\2_Semestre\Programacao_II\Praticas\Ficha1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F4A2E9-44D6-46DB-BC41-FCAB5F8FA68B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha 1" sheetId="29" r:id="rId1"/>
+    <sheet name="Original" sheetId="30" r:id="rId1"/>
+    <sheet name="Ficha1" sheetId="29" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Atributos</t>
   </si>
@@ -35,12 +37,72 @@
   <si>
     <t>SuperClasses/Interfaces</t>
   </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Aluno</t>
+  </si>
+  <si>
+    <t>Aula</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>aulas</t>
+  </si>
+  <si>
+    <t>LinkedList&lt;Aula&gt;</t>
+  </si>
+  <si>
+    <t>preencherSumario(Aula)</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>adicionar(Aula)</t>
+  </si>
+  <si>
+    <t>sumario</t>
+  </si>
+  <si>
+    <t>alunos</t>
+  </si>
+  <si>
+    <t>professor</t>
+  </si>
+  <si>
+    <t>LinkedList&lt;Aluno&gt;</t>
+  </si>
+  <si>
+    <t>adicionarLinhaSumario(String)</t>
+  </si>
+  <si>
+    <t>atribuir(Professor)</t>
+  </si>
+  <si>
+    <t>adicionar(Aluno)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -69,6 +131,21 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
@@ -135,7 +212,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -143,7 +220,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -163,7 +240,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -253,7 +336,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -572,21 +655,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A2E451-5FF5-4460-B671-6A94535E6752}">
   <dimension ref="A1:AD213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="30" width="3.6640625" style="5" customWidth="1"/>
-    <col min="31" max="16384" width="8.6640625" style="5"/>
+    <col min="1" max="2" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="30" width="3.7109375" style="5" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -620,7 +703,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="95.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -656,7 +739,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -690,7 +773,7 @@
       <c r="AC3" s="9"/>
       <c r="AD3" s="9"/>
     </row>
-    <row r="4" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
@@ -722,7 +805,7 @@
       <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
     </row>
-    <row r="5" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
@@ -754,7 +837,7 @@
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
     </row>
-    <row r="6" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
@@ -786,7 +869,7 @@
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
     </row>
-    <row r="7" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -818,12 +901,1051 @@
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
     </row>
-    <row r="8" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+    </row>
+    <row r="9" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+    </row>
+    <row r="10" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+    </row>
+    <row r="11" spans="1:30" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+    </row>
+    <row r="12" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+    </row>
+    <row r="13" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+    </row>
+    <row r="14" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+    </row>
+    <row r="15" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+    </row>
+    <row r="16" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+    </row>
+    <row r="17" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+    </row>
+    <row r="18" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+    </row>
+    <row r="19" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+    </row>
+    <row r="20" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+    </row>
+    <row r="21" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+    </row>
+    <row r="22" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+    </row>
+    <row r="23" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+    </row>
+    <row r="24" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+    </row>
+    <row r="25" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+    </row>
+    <row r="26" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
+    </row>
+    <row r="27" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD213"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="30" width="3.7109375" style="5" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+    </row>
+    <row r="2" spans="1:30" ht="95.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+    </row>
+    <row r="3" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+    </row>
+    <row r="4" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+    </row>
+    <row r="5" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+    </row>
+    <row r="6" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+    </row>
+    <row r="7" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+    </row>
+    <row r="8" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -850,12 +1972,18 @@
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
-    <row r="9" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+    <row r="9" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -882,7 +2010,7 @@
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
     </row>
-    <row r="10" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -894,7 +2022,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="L10" s="13"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
@@ -914,7 +2042,7 @@
       <c r="AC10" s="11"/>
       <c r="AD10" s="11"/>
     </row>
-    <row r="11" spans="1:30" ht="10.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -946,7 +2074,7 @@
       <c r="AC11" s="11"/>
       <c r="AD11" s="11"/>
     </row>
-    <row r="12" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -978,7 +2106,7 @@
       <c r="AC12" s="11"/>
       <c r="AD12" s="11"/>
     </row>
-    <row r="13" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -1010,7 +2138,7 @@
       <c r="AC13" s="11"/>
       <c r="AD13" s="11"/>
     </row>
-    <row r="14" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -1042,7 +2170,7 @@
       <c r="AC14" s="11"/>
       <c r="AD14" s="11"/>
     </row>
-    <row r="15" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
@@ -1074,7 +2202,7 @@
       <c r="AC15" s="11"/>
       <c r="AD15" s="11"/>
     </row>
-    <row r="16" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
         <v>1</v>
@@ -1108,11 +2236,19 @@
       <c r="AC16" s="9"/>
       <c r="AD16" s="9"/>
     </row>
-    <row r="17" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+    <row r="17" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -1140,11 +2276,19 @@
       <c r="AC17" s="11"/>
       <c r="AD17" s="11"/>
     </row>
-    <row r="18" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+    <row r="18" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -1172,12 +2316,18 @@
       <c r="AC18" s="11"/>
       <c r="AD18" s="11"/>
     </row>
-    <row r="19" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+    <row r="19" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -1204,12 +2354,18 @@
       <c r="AC19" s="11"/>
       <c r="AD19" s="11"/>
     </row>
-    <row r="20" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+    <row r="20" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -1236,12 +2392,18 @@
       <c r="AC20" s="11"/>
       <c r="AD20" s="11"/>
     </row>
-    <row r="21" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+    <row r="21" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -1268,7 +2430,7 @@
       <c r="AC21" s="11"/>
       <c r="AD21" s="11"/>
     </row>
-    <row r="22" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -1300,7 +2462,7 @@
       <c r="AC22" s="11"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="23" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -1332,7 +2494,7 @@
       <c r="AC23" s="11"/>
       <c r="AD23" s="11"/>
     </row>
-    <row r="24" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
@@ -1364,7 +2526,7 @@
       <c r="AC24" s="11"/>
       <c r="AD24" s="11"/>
     </row>
-    <row r="25" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -1396,7 +2558,7 @@
       <c r="AC25" s="11"/>
       <c r="AD25" s="11"/>
     </row>
-    <row r="26" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -1428,193 +2590,193 @@
       <c r="AC26" s="11"/>
       <c r="AD26" s="11"/>
     </row>
-    <row r="27" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>